<commit_message>
fix: clean up sheet
</commit_message>
<xml_diff>
--- a/solar_gmbh_management_report.xlsx
+++ b/solar_gmbh_management_report.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="255" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78750F82-359A-4D7C-BD0E-1D23CAA47230}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/git/solar_analyst_exercise/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE582F59-C378-DD47-9892-6657FE40868A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="760" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;L" sheetId="1" r:id="rId1"/>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>Account</t>
   </si>
@@ -102,6 +107,9 @@
   </si>
   <si>
     <t>Installation</t>
+  </si>
+  <si>
+    <t>Cost Cetner</t>
   </si>
 </sst>
 </file>
@@ -109,9 +117,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_([$€-2]\ * #,##0_);_([$€-2]\ * \(#,##0\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_([$€-2]\ * #,##0_);_([$€-2]\ * \(#,##0\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +133,13 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -148,10 +163,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,246 +502,246 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2">
+      <c r="B2" s="2">
         <f>SUM('Sales by Product'!B2:B4)</f>
         <v>700000</v>
       </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2">
         <f>SUM('Sales by Product'!C2:C4)</f>
         <v>1030000</v>
       </c>
-      <c r="E2" s="2">
+      <c r="D2" s="2">
         <f>SUM('Sales by Product'!D2:D4)</f>
         <v>1075000</v>
       </c>
-      <c r="F2" s="2">
+      <c r="E2" s="2">
         <f>SUM('Sales by Product'!E2:E4)</f>
         <v>1125000</v>
       </c>
-      <c r="G2" s="2">
+      <c r="F2" s="2">
         <f>SUM('Sales by Product'!F2:F4)</f>
         <v>1350000</v>
       </c>
-      <c r="H2" s="2">
+      <c r="G2" s="2">
         <f>SUM('Sales by Product'!G2:G4)</f>
         <v>1550000</v>
       </c>
-      <c r="I2" s="2">
+      <c r="H2" s="2">
         <f>SUM('Sales by Product'!H2:H4)</f>
         <v>1850000</v>
       </c>
-      <c r="J2" s="2">
+      <c r="I2" s="2">
         <f>SUM('Sales by Product'!I2:I4)</f>
         <v>2120000</v>
       </c>
-      <c r="K2" s="2">
+      <c r="J2" s="2">
         <f>SUM('Sales by Product'!J2:J4)</f>
         <v>1230000</v>
       </c>
-      <c r="L2" s="2">
+      <c r="K2" s="2">
         <f>SUM('Sales by Product'!K2:K4)</f>
         <v>940000</v>
       </c>
-      <c r="M2" s="2">
+      <c r="L2" s="2">
         <f>SUM('Sales by Product'!L2:L4)</f>
         <v>650000</v>
       </c>
-      <c r="N2" s="2">
+      <c r="M2" s="2">
         <f>SUM('Sales by Product'!M2:M4)</f>
         <v>500000</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2">
+      <c r="B3" s="2">
         <f>SUM('Salaries by Cost Center'!B2:B4)</f>
         <v>140000</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
         <f>SUM('Salaries by Cost Center'!C2:C4)</f>
         <v>140000</v>
       </c>
-      <c r="E3" s="2">
+      <c r="D3" s="2">
         <f>SUM('Salaries by Cost Center'!D2:D4)</f>
         <v>140000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="E3" s="2">
         <f>SUM('Salaries by Cost Center'!E2:E4)</f>
         <v>140000</v>
       </c>
-      <c r="G3" s="2">
+      <c r="F3" s="2">
         <f>SUM('Salaries by Cost Center'!F2:F4)</f>
         <v>140000</v>
       </c>
-      <c r="H3" s="2">
+      <c r="G3" s="2">
         <f>SUM('Salaries by Cost Center'!G2:G4)</f>
         <v>181000</v>
       </c>
-      <c r="I3" s="2">
+      <c r="H3" s="2">
         <f>SUM('Salaries by Cost Center'!H2:H4)</f>
         <v>181000</v>
       </c>
-      <c r="J3" s="2">
+      <c r="I3" s="2">
         <f>SUM('Salaries by Cost Center'!I2:I4)</f>
         <v>181000</v>
       </c>
-      <c r="K3" s="2">
+      <c r="J3" s="2">
         <f>SUM('Salaries by Cost Center'!J2:J4)</f>
         <v>181000</v>
       </c>
-      <c r="L3" s="2">
+      <c r="K3" s="2">
         <f>SUM('Salaries by Cost Center'!K2:K4)</f>
         <v>181000</v>
       </c>
-      <c r="M3" s="2">
+      <c r="L3" s="2">
         <f>SUM('Salaries by Cost Center'!L2:L4)</f>
         <v>181000</v>
       </c>
-      <c r="N3" s="2">
+      <c r="M3" s="2">
         <f>SUM('Salaries by Cost Center'!M2:M4)</f>
         <v>181000</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B4" s="2">
+        <v>650000</v>
+      </c>
       <c r="C4" s="2">
+        <v>800000</v>
+      </c>
+      <c r="D4" s="2">
+        <v>860000</v>
+      </c>
+      <c r="E4" s="2">
+        <v>950000</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1200000</v>
+      </c>
+      <c r="G4" s="2">
+        <v>850000</v>
+      </c>
+      <c r="H4" s="2">
+        <v>900000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>800000</v>
+      </c>
+      <c r="J4" s="2">
+        <v>700000</v>
+      </c>
+      <c r="K4" s="2">
         <v>650000</v>
       </c>
-      <c r="D4" s="2">
-        <v>800000</v>
-      </c>
-      <c r="E4" s="2">
-        <v>860000</v>
-      </c>
-      <c r="F4" s="2">
-        <v>950000</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1200000</v>
-      </c>
-      <c r="H4" s="2">
-        <v>850000</v>
-      </c>
-      <c r="I4" s="2">
-        <v>900000</v>
-      </c>
-      <c r="J4" s="2">
-        <v>800000</v>
-      </c>
-      <c r="K4" s="2">
-        <v>700000</v>
-      </c>
       <c r="L4" s="2">
-        <v>650000</v>
+        <v>600000</v>
       </c>
       <c r="M4" s="2">
-        <v>600000</v>
-      </c>
-      <c r="N4" s="2">
         <v>500000</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B5" s="2">
+        <v>2000</v>
+      </c>
       <c r="C5" s="2">
         <v>2000</v>
       </c>
       <c r="D5" s="2">
+        <v>54000</v>
+      </c>
+      <c r="E5" s="2">
         <v>2000</v>
-      </c>
-      <c r="E5" s="2">
-        <v>54000</v>
       </c>
       <c r="F5" s="2">
         <v>2000</v>
       </c>
       <c r="G5" s="2">
-        <v>2000</v>
+        <v>64000</v>
       </c>
       <c r="H5" s="2">
-        <v>64000</v>
+        <v>2500</v>
       </c>
       <c r="I5" s="2">
         <v>2500</v>
       </c>
       <c r="J5" s="2">
+        <v>65000</v>
+      </c>
+      <c r="K5" s="2">
         <v>2500</v>
-      </c>
-      <c r="K5" s="2">
-        <v>65000</v>
       </c>
       <c r="L5" s="2">
         <v>2500</v>
       </c>
       <c r="M5" s="2">
-        <v>2500</v>
-      </c>
-      <c r="N5" s="2">
         <v>65000</v>
       </c>
     </row>
@@ -739,18 +755,18 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="13.5" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -791,8 +807,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="2">
@@ -832,8 +848,8 @@
         <v>255000</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="2">
@@ -873,8 +889,8 @@
         <v>125000</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="2">
@@ -923,18 +939,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107D44A9-934D-4306-8BA1-58044CD69406}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -972,8 +991,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2">
@@ -1013,8 +1032,8 @@
         <v>111000</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="2">
@@ -1054,8 +1073,8 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="2">

</xml_diff>

<commit_message>
fix: remove number formatting
</commit_message>
<xml_diff>
--- a/solar_gmbh_management_report.xlsx
+++ b/solar_gmbh_management_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/git/solar_analyst_exercise/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE582F59-C378-DD47-9892-6657FE40868A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D5C873-BEEC-304B-9D99-610873BC24BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="760" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;L" sheetId="1" r:id="rId1"/>
@@ -109,16 +109,13 @@
     <t>Installation</t>
   </si>
   <si>
-    <t>Cost Cetner</t>
+    <t>Cost Center</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_([$€-2]\ * #,##0_);_([$€-2]\ * \(#,##0\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,7 +163,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -502,246 +499,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="2">
         <f>SUM('Sales by Product'!B2:B4)</f>
         <v>700000</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <f>SUM('Sales by Product'!C2:C4)</f>
         <v>1030000</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <f>SUM('Sales by Product'!D2:D4)</f>
         <v>1075000</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <f>SUM('Sales by Product'!E2:E4)</f>
         <v>1125000</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <f>SUM('Sales by Product'!F2:F4)</f>
         <v>1350000</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <f>SUM('Sales by Product'!G2:G4)</f>
         <v>1550000</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <f>SUM('Sales by Product'!H2:H4)</f>
         <v>1850000</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <f>SUM('Sales by Product'!I2:I4)</f>
         <v>2120000</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <f>SUM('Sales by Product'!J2:J4)</f>
         <v>1230000</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <f>SUM('Sales by Product'!K2:K4)</f>
         <v>940000</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <f>SUM('Sales by Product'!L2:L4)</f>
         <v>650000</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <f>SUM('Sales by Product'!M2:M4)</f>
         <v>500000</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="2">
         <f>SUM('Salaries by Cost Center'!B2:B4)</f>
         <v>140000</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <f>SUM('Salaries by Cost Center'!C2:C4)</f>
         <v>140000</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <f>SUM('Salaries by Cost Center'!D2:D4)</f>
         <v>140000</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <f>SUM('Salaries by Cost Center'!E2:E4)</f>
         <v>140000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <f>SUM('Salaries by Cost Center'!F2:F4)</f>
         <v>140000</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <f>SUM('Salaries by Cost Center'!G2:G4)</f>
         <v>181000</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <f>SUM('Salaries by Cost Center'!H2:H4)</f>
         <v>181000</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <f>SUM('Salaries by Cost Center'!I2:I4)</f>
         <v>181000</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <f>SUM('Salaries by Cost Center'!J2:J4)</f>
         <v>181000</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <f>SUM('Salaries by Cost Center'!K2:K4)</f>
         <v>181000</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <f>SUM('Salaries by Cost Center'!L2:L4)</f>
         <v>181000</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <f>SUM('Salaries by Cost Center'!M2:M4)</f>
         <v>181000</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="2">
         <v>650000</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>800000</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>860000</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>950000</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>1200000</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>850000</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>900000</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>800000</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>700000</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>650000</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>600000</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>500000</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2">
-        <v>2000</v>
-      </c>
       <c r="C5" s="2">
         <v>2000</v>
       </c>
       <c r="D5" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E5" s="2">
         <v>54000</v>
-      </c>
-      <c r="E5" s="2">
-        <v>2000</v>
       </c>
       <c r="F5" s="2">
         <v>2000</v>
       </c>
       <c r="G5" s="2">
+        <v>2000</v>
+      </c>
+      <c r="H5" s="2">
         <v>64000</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2500</v>
       </c>
       <c r="I5" s="2">
         <v>2500</v>
       </c>
       <c r="J5" s="2">
+        <v>2500</v>
+      </c>
+      <c r="K5" s="2">
         <v>65000</v>
-      </c>
-      <c r="K5" s="2">
-        <v>2500</v>
       </c>
       <c r="L5" s="2">
         <v>2500</v>
       </c>
       <c r="M5" s="2">
+        <v>2500</v>
+      </c>
+      <c r="N5" s="2">
         <v>65000</v>
       </c>
     </row>
@@ -754,9 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A204B188-4FC8-41B6-A552-CB53B84FE9FB}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -808,7 +801,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="2">
@@ -849,7 +842,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="2">
@@ -890,7 +883,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="2">
@@ -939,9 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107D44A9-934D-4306-8BA1-58044CD69406}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>